<commit_message>
Correzioni a valle del Manuale. Problemi con ONR (stiamo lavorandoci su...)
</commit_message>
<xml_diff>
--- a/set_anomalie.xlsx
+++ b/set_anomalie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\PycharmProjects\ARStool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95726910-D884-4C0F-9130-C07FF7A8F987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8117D517-492D-446E-9C40-941FA0DCF3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5475" windowWidth="38640" windowHeight="21240" xr2:uid="{46984E79-C21C-4C6B-AAA7-DC7D1D989A26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46984E79-C21C-4C6B-AAA7-DC7D1D989A26}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +193,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -304,10 +311,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -315,7 +321,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -653,7 +661,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,76 +676,76 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -751,39 +759,27 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>0.3</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="3"/>
+      <c r="T2" s="2"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="3"/>
+      <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -795,39 +791,27 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>15</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>0.3</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="3"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="1"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="3"/>
+      <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -837,29 +821,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="3"/>
+      <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -869,29 +837,13 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="3"/>
+      <c r="T5" s="2"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="3"/>
+      <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -901,29 +853,13 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="2"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="3"/>
+      <c r="T6" s="2"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="3"/>
+      <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -933,29 +869,13 @@
         <v>34</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
+      <c r="N7" s="2"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="3"/>
+      <c r="T7" s="2"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="3"/>
+      <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -967,47 +887,37 @@
       <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>1.5</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>0.5</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8">
         <v>1095</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
         <v>3</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>0.7</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="3"/>
+      <c r="T8" s="2"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="3"/>
+      <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1019,37 +929,24 @@
       <c r="C9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>1095</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>0.7</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="2"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="3"/>
+      <c r="T9" s="2"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="3"/>
+      <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1058,46 +955,34 @@
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="10">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="10">
         <v>4</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3">
+      <c r="G10" s="10"/>
+      <c r="H10" s="11">
         <v>0.5</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
+      <c r="N10" s="2"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="3"/>
+      <c r="T10" s="2"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="3"/>
+      <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -1109,38 +994,29 @@
       <c r="F11" s="10">
         <v>4</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="3">
+      <c r="G11" s="10"/>
+      <c r="H11" s="11">
         <v>0.5</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11">
         <v>1.5</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>0.5</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="3"/>
+      <c r="T11" s="2"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="3"/>
+      <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1150,29 +1026,13 @@
         <v>34</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="2"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="3"/>
+      <c r="T12" s="2"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="3"/>
+      <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1184,453 +1044,200 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13">
         <v>5</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>0.3</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
+      <c r="N13" s="2"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="3"/>
+      <c r="T13" s="2"/>
       <c r="U13" s="1"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="3"/>
+      <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="2"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="3"/>
+      <c r="N14" s="2"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="3"/>
+      <c r="T14" s="2"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="3"/>
+      <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="2"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
+      <c r="N15" s="2"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="3"/>
+      <c r="T15" s="2"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="3"/>
+      <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="2"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
+      <c r="N16" s="2"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="3"/>
+      <c r="T16" s="2"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="3"/>
+      <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="2"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
+      <c r="N17" s="2"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="3"/>
+      <c r="T17" s="2"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="3"/>
+      <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="2"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="3"/>
+      <c r="T18" s="2"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="3"/>
+      <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
+      <c r="N19" s="2"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="3"/>
+      <c r="T19" s="2"/>
       <c r="U19" s="1"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="3"/>
+      <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="2"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="3"/>
+      <c r="N20" s="2"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="3"/>
+      <c r="T20" s="2"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="3"/>
+      <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
+      <c r="N21" s="2"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="3"/>
+      <c r="T21" s="2"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="3"/>
+      <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
+      <c r="N22" s="2"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="3"/>
+      <c r="T22" s="2"/>
       <c r="U22" s="1"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="3"/>
+      <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="2"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
+      <c r="N23" s="2"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="3"/>
+      <c r="T23" s="2"/>
       <c r="U23" s="1"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-      <c r="Z23" s="3"/>
+      <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="2"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
+      <c r="N24" s="2"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="3"/>
+      <c r="T24" s="2"/>
       <c r="U24" s="1"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="3"/>
+      <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="2"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="3"/>
+      <c r="T25" s="2"/>
       <c r="U25" s="1"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="3"/>
+      <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="2"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
+      <c r="N26" s="2"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="3"/>
+      <c r="T26" s="2"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="3"/>
+      <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="3"/>
+      <c r="N27" s="2"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="3"/>
+      <c r="T27" s="2"/>
       <c r="U27" s="1"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="3"/>
+      <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
+      <c r="H28" s="2"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="2"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="3"/>
+      <c r="T28" s="2"/>
       <c r="U28" s="1"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="3"/>
+      <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="6"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>